<commit_message>
Refactoring internal API for common resources
</commit_message>
<xml_diff>
--- a/test/xlsx/images.xlsx
+++ b/test/xlsx/images.xlsx
@@ -5,8 +5,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1" state="visible"/>
-    <sheet name="Sheet 2" sheetId="2" r:id="rId2" state="visible"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId2" state="visible"/>
+    <sheet name="Sheet 2" sheetId="2" r:id="rId3" state="visible"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>